<commit_message>
ajout du code de l'exo avec Linq
</commit_message>
<xml_diff>
--- a/personnel/marché/Place du marché.xlsx
+++ b/personnel/marché/Place du marché.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pf25xeu\Documents\GitHub\323-Programmation_fonctionnelle\personnel\marché\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DBA351-1E09-4547-BD5C-5A33785789A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC76971C-439B-4F99-94D9-9F834F406E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>